<commit_message>
includes addSpecies function to 12s workup
</commit_message>
<xml_diff>
--- a/Deliverables/marker_species_proportions.xlsx
+++ b/Deliverables/marker_species_proportions.xlsx
@@ -1,35 +1,164 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intern\Arctic-predator-diet-microbiome\Deliverables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108"/>
   </bookViews>
   <sheets>
-    <sheet name="12s" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="16s" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="12S" sheetId="1" r:id="rId1"/>
+    <sheet name="16S" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">Marker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Species</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prop_abundance</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+  <si>
+    <t>Marker</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>prop_abundance</t>
+  </si>
+  <si>
+    <t>12S</t>
+  </si>
+  <si>
+    <t>Clupea pallasii</t>
+  </si>
+  <si>
+    <t>Gadus chalcogrammus</t>
+  </si>
+  <si>
+    <t>Artedius harringtoni</t>
+  </si>
+  <si>
+    <t>Chitonotus pugetensis</t>
+  </si>
+  <si>
+    <t>Gymnelus viridis</t>
+  </si>
+  <si>
+    <t>Ophiodon elongatus</t>
+  </si>
+  <si>
+    <t>Stenobrachius leucopsarus</t>
+  </si>
+  <si>
+    <t>Oncorhynchus kisutch</t>
+  </si>
+  <si>
+    <t>Liparis spp.</t>
+  </si>
+  <si>
+    <t>Citharichthys sordidus</t>
+  </si>
+  <si>
+    <t>Hypomesus olidus</t>
+  </si>
+  <si>
+    <t>Gymnocanthus spp.</t>
+  </si>
+  <si>
+    <t>Pungitius pungitius</t>
+  </si>
+  <si>
+    <t>Coregonus laurettae</t>
+  </si>
+  <si>
+    <t>Melanogrammus aeglefinus</t>
+  </si>
+  <si>
+    <t>Eleginus gracilis</t>
+  </si>
+  <si>
+    <t>Chesnonia verrucosa</t>
+  </si>
+  <si>
+    <t>Ammodytes personatus</t>
+  </si>
+  <si>
+    <t>Mallotus villosus</t>
+  </si>
+  <si>
+    <t>Coregonus spp.</t>
+  </si>
+  <si>
+    <t>Ammodytes spp.</t>
+  </si>
+  <si>
+    <t>Lumpenus sagitta</t>
+  </si>
+  <si>
+    <t>Myoxocephalus spp.</t>
+  </si>
+  <si>
+    <t>Osmerus mordax</t>
+  </si>
+  <si>
+    <t>Gasterosteus aculeatus</t>
+  </si>
+  <si>
+    <t>Clupea spp.</t>
+  </si>
+  <si>
+    <t>Aspidophoroides monopterygius</t>
+  </si>
+  <si>
+    <t>16S</t>
+  </si>
+  <si>
+    <t>Microcottus sellaris</t>
+  </si>
+  <si>
+    <t>Ammodytes hexapterus</t>
+  </si>
+  <si>
+    <t>Limanda aspera</t>
+  </si>
+  <si>
+    <t>Oncorhynchus keta</t>
+  </si>
+  <si>
+    <t>Stichaeus punctatus</t>
+  </si>
+  <si>
+    <t>Parophrys vetulus</t>
+  </si>
+  <si>
+    <t>Gymnocanthus tricuspis</t>
+  </si>
+  <si>
+    <t>Gymnocanthus pistilliger</t>
+  </si>
+  <si>
+    <t>Pallasina barbata</t>
+  </si>
+  <si>
+    <t>Esox lucius</t>
+  </si>
+  <si>
+    <t>Salvelinus spp.</t>
+  </si>
+  <si>
+    <t>total equal to:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -65,6 +194,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -346,14 +484,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -364,21 +508,333 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>0.51569895575492697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>9.5666557956236103E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>4.99119661805658E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>4.99119661805658E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>4.99119661805658E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>4.99119661805658E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>4.99119661805658E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>4.8690878322937302E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>3.79066134598008E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>2.49559830902829E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1.22431327863408E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>7.7987205718161E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>3.5487210781209302E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>1.1174320786693801E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>9.7675080588191109E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>5.2245936632843598E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>3.0102710378629102E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>2.9994127037615698E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>2.9676382716055502E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>1.87473138548303E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>1.3227552874708201E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>7.16097075761347E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>1.11113014649523E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>9.4674958397889301E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>4.0506470359146603E-6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>2.4380529453589799E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <f>SUM(C2:C28)</f>
+        <v>1.0000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21:D21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +845,215 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>0.45241657511826899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0.147592603538892</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>7.1236226964228697E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>6.3912256525738398E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>6.3912256525738398E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>6.3590894067257597E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>5.5839330306785499E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>2.3557402245063801E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>2.0895301358046198E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>1.3563276776715E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12">
+        <v>7.6610750843659897E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13">
+        <v>5.0127983699793204E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>3.6802536000526999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>3.1810179576594998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16">
+        <v>2.6330906365178899E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17">
+        <v>7.0862707041380497E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>3.5492066889422901E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>2.5209318538281701E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <f>SUM(C2:C19)</f>
+        <v>1.0000000000000007</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>